<commit_message>
Modificacion sobre concentrado de metricas Abril
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150430.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150430.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -224,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +264,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +461,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -478,9 +496,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -537,18 +552,37 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="97">
@@ -650,161 +684,7 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="86">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="64">
     <dxf>
       <fill>
         <patternFill>
@@ -1367,10 +1247,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>140</c:v>
+                  <c:v>91.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45.600000000000009</c:v>
@@ -1495,11 +1375,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5403632"/>
-        <c:axId val="5404192"/>
+        <c:axId val="345137904"/>
+        <c:axId val="345138464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5403632"/>
+        <c:axId val="345137904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1389,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5404192"/>
+        <c:crossAx val="345138464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1517,7 +1397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5404192"/>
+        <c:axId val="345138464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,7 +1408,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5403632"/>
+        <c:crossAx val="345137904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1644,11 +1524,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="165081840"/>
-        <c:axId val="165082400"/>
+        <c:axId val="398206688"/>
+        <c:axId val="398207248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165081840"/>
+        <c:axId val="398206688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1538,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165082400"/>
+        <c:crossAx val="398207248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1666,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165082400"/>
+        <c:axId val="398207248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1678,7 +1558,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165081840"/>
+        <c:crossAx val="398206688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,11 +1782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191761472"/>
-        <c:axId val="191762032"/>
+        <c:axId val="398583264"/>
+        <c:axId val="295112224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191761472"/>
+        <c:axId val="398583264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,7 +1796,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191762032"/>
+        <c:crossAx val="295112224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1924,7 +1804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191762032"/>
+        <c:axId val="295112224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1936,7 +1816,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191761472"/>
+        <c:crossAx val="398583264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2070,10 +1950,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.76428571428571423</c:v>
+                  <c:v>0.63815789473684215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90714285714285714</c:v>
+                  <c:v>0.71491228070175439</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.62719298245614041</c:v>
@@ -2108,11 +1988,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5406992"/>
-        <c:axId val="5407552"/>
+        <c:axId val="290162272"/>
+        <c:axId val="290162832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5406992"/>
+        <c:axId val="290162272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2122,7 +2002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5407552"/>
+        <c:crossAx val="290162832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2130,7 +2010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5407552"/>
+        <c:axId val="290162832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2143,7 +2023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5406992"/>
+        <c:crossAx val="290162272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2236,7 +2116,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11653</c:v>
+                  <c:v>9989</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5693.7300000000005</c:v>
@@ -2286,7 +2166,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4979.0600000000004</c:v>
+                  <c:v>1914.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1984.52</c:v>
@@ -2309,11 +2189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5410352"/>
-        <c:axId val="106299248"/>
+        <c:axId val="290165632"/>
+        <c:axId val="294236128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5410352"/>
+        <c:axId val="290165632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2203,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106299248"/>
+        <c:crossAx val="294236128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2331,7 +2211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106299248"/>
+        <c:axId val="294236128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2342,7 +2222,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5410352"/>
+        <c:crossAx val="290165632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2440,7 +2320,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.57272290397322578</c:v>
+                  <c:v>0.80833717088797674</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.65145519720815703</c:v>
@@ -2463,11 +2343,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106302048"/>
-        <c:axId val="106302608"/>
+        <c:axId val="294238928"/>
+        <c:axId val="294239488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106302048"/>
+        <c:axId val="294238928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,7 +2357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106302608"/>
+        <c:crossAx val="294239488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2485,7 +2365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106302608"/>
+        <c:axId val="294239488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2498,7 +2378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106302048"/>
+        <c:crossAx val="294238928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2609,11 +2489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106304848"/>
-        <c:axId val="106305408"/>
+        <c:axId val="296834528"/>
+        <c:axId val="296835088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106304848"/>
+        <c:axId val="296834528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2623,7 +2503,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106305408"/>
+        <c:crossAx val="296835088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2631,7 +2511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106305408"/>
+        <c:axId val="296835088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2642,7 +2522,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106304848"/>
+        <c:crossAx val="296834528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2759,11 +2639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164856784"/>
-        <c:axId val="164857344"/>
+        <c:axId val="294936480"/>
+        <c:axId val="294937040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164856784"/>
+        <c:axId val="294936480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2653,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164857344"/>
+        <c:crossAx val="294937040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2781,7 +2661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164857344"/>
+        <c:axId val="294937040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2793,7 +2673,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164856784"/>
+        <c:crossAx val="294936480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2916,11 +2796,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164860144"/>
-        <c:axId val="164860704"/>
+        <c:axId val="104260080"/>
+        <c:axId val="104260640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164860144"/>
+        <c:axId val="104260080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +2810,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164860704"/>
+        <c:crossAx val="104260640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2938,7 +2818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164860704"/>
+        <c:axId val="104260640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2950,7 +2830,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164860144"/>
+        <c:crossAx val="104260080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3067,11 +2947,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="165075120"/>
-        <c:axId val="165075680"/>
+        <c:axId val="288223312"/>
+        <c:axId val="288223872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165075120"/>
+        <c:axId val="288223312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3081,7 +2961,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165075680"/>
+        <c:crossAx val="288223872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3089,7 +2969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165075680"/>
+        <c:axId val="288223872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3101,7 +2981,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165075120"/>
+        <c:crossAx val="288223312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3218,11 +3098,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="165078480"/>
-        <c:axId val="165079040"/>
+        <c:axId val="288226672"/>
+        <c:axId val="398203888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165078480"/>
+        <c:axId val="288226672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3232,7 +3112,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165079040"/>
+        <c:crossAx val="398203888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3240,7 +3120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165079040"/>
+        <c:axId val="398203888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3252,7 +3132,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165078480"/>
+        <c:crossAx val="288226672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3295,7 +3175,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3331,7 +3211,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3374,7 +3254,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3412,7 +3292,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3455,7 +3335,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3491,7 +3371,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3532,7 +3412,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3568,7 +3448,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3609,7 +3489,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3652,7 +3532,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3999,8 +3879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F26" sqref="B19:F26"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,131 +3916,131 @@
     <row r="17" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="38">
-        <v>140</v>
-      </c>
-      <c r="E20" s="38">
+      <c r="D20" s="37">
+        <v>91.2</v>
+      </c>
+      <c r="E20" s="37">
         <v>33</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="41">
         <f>(D20-E20)/D20</f>
-        <v>0.76428571428571423</v>
+        <v>0.63815789473684215</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="38">
-        <v>140</v>
-      </c>
-      <c r="E21" s="38">
+      <c r="D21" s="37">
+        <v>45.6</v>
+      </c>
+      <c r="E21" s="37">
         <v>13</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="42">
         <f t="shared" ref="F21:F26" si="0">(D21-E21)/D21</f>
-        <v>0.90714285714285714</v>
+        <v>0.71491228070175439</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="37">
         <v>45.600000000000009</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="37">
         <v>17</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="41">
         <f t="shared" si="0"/>
         <v>0.62719298245614041</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41"/>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="37">
         <v>91.200000000000017</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="37">
         <v>28</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="42">
         <f t="shared" si="0"/>
         <v>0.69298245614035092</v>
       </c>
     </row>
     <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37">
+      <c r="C24" s="35"/>
+      <c r="D24" s="36">
         <v>1</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="36">
         <v>1</v>
       </c>
-      <c r="F24" s="42">
+      <c r="F24" s="43">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37">
+      <c r="C25" s="35"/>
+      <c r="D25" s="36">
         <v>2</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="36">
         <v>1.6</v>
       </c>
-      <c r="F25" s="42">
+      <c r="F25" s="43">
         <f t="shared" si="0"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37">
+      <c r="C26" s="35"/>
+      <c r="D26" s="36">
         <v>0.5</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="39">
         <v>0.17</v>
       </c>
-      <c r="F26" s="42">
+      <c r="F26" s="44">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4649,7 +4529,7 @@
     <mergeCell ref="B20:B21"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:XFD1048576">
-    <cfRule type="cellIs" dxfId="85" priority="63" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="63" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4669,7 +4549,7 @@
   <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4723,14 +4603,14 @@
         <v>3</v>
       </c>
       <c r="C20" s="15">
-        <v>11653</v>
+        <v>9989</v>
       </c>
       <c r="D20" s="15">
-        <v>4979.0600000000004</v>
-      </c>
-      <c r="E20" s="16">
+        <v>1914.52</v>
+      </c>
+      <c r="E20" s="45">
         <f>(C20-D20)/C20</f>
-        <v>0.57272290397322578</v>
+        <v>0.80833717088797674</v>
       </c>
     </row>
     <row r="21" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4743,7 +4623,7 @@
       <c r="D21" s="15">
         <v>1984.52</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="46">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.65145519720815703</v>
       </c>
@@ -4760,7 +4640,7 @@
     <row r="31" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A27:XFD1048576">
-    <cfRule type="cellIs" dxfId="84" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4776,7 +4656,7 @@
   <dimension ref="B2:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4796,94 +4676,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150330</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>1</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>1</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="47">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>0.8</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>1</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="47">
         <f>AVERAGE(D5:F5)</f>
         <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="26" t="e">
+      <c r="G6" s="25" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4893,91 +4773,91 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>7</v>
       </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="30">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="29">
         <v>150227</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>150331</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>150330</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="26"/>
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="28" t="e">
+      <c r="F10" s="23"/>
+      <c r="G10" s="27" t="e">
         <f t="shared" ref="G10:G12" si="0">AVERAGE(D10:F10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="28" t="e">
+      <c r="F11" s="23"/>
+      <c r="G11" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="28" t="e">
+      <c r="F12" s="23"/>
+      <c r="G12" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -4985,77 +4865,77 @@
     <row r="25" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A3:C3 M2:XFD6 A9:A12 A15:XFD1048576 A8:B8 A4:G6 A2:E2 A7:H7 H8 A13:H14 J7:XFD14 G9:H12 G2">
-    <cfRule type="cellIs" dxfId="83" priority="22" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="82" priority="18" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="81" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="80" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="79" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F12">
-    <cfRule type="cellIs" dxfId="78" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C12">
-    <cfRule type="cellIs" dxfId="77" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="55" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="75" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="74" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="73" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="72" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="71" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5075,7 +4955,7 @@
   <dimension ref="B2:I40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,56 +4973,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150330</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="48">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5150,22 +5030,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="48">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5173,22 +5053,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>1</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <v>1</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>1</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="48">
         <f>AVERAGE(D6:F6)</f>
         <v>1</v>
       </c>
@@ -5196,22 +5076,22 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>1</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="48">
         <f>AVERAGE(D7:F7)</f>
         <v>1</v>
       </c>
@@ -5219,67 +5099,67 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="30">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="29">
         <v>150227</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>150331</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>150330</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>1</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="26" t="e">
+      <c r="G11" s="25" t="e">
         <f t="shared" ref="G11:G13" si="0">AVERAGE(D11:F11)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5287,22 +5167,22 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="26" t="e">
+      <c r="G12" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5310,22 +5190,22 @@
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="26" t="e">
+      <c r="G13" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5367,117 +5247,117 @@
     <sortCondition descending="1" ref="C29"/>
   </sortState>
   <conditionalFormatting sqref="J2:XFD11 A2:A12 H2:I3 H12:XFD12 A14:XFD15 A19:XFD1048576 A16:B18 D16:XFD18">
-    <cfRule type="cellIs" dxfId="69" priority="32" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="32" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B9 B2:D2 G10:G13 C4:G6 G2">
-    <cfRule type="cellIs" dxfId="68" priority="31" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="31" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="67" priority="28" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="28" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="66" priority="29" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="29" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="64" priority="22" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D13">
-    <cfRule type="cellIs" dxfId="63" priority="26" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="26" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="62" priority="25" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="25" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C13">
-    <cfRule type="cellIs" dxfId="61" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="60" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="cellIs" dxfId="59" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:F13">
-    <cfRule type="cellIs" dxfId="56" priority="16" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="55" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="54" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="53" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="52" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="51" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="50" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:G8">
-    <cfRule type="cellIs" dxfId="49" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="cellIs" dxfId="48" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5496,7 +5376,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5514,56 +5394,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150330</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="48">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5571,22 +5451,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="48">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5594,22 +5474,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="28" t="e">
+      <c r="G6" s="27" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5655,42 +5535,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:XFD7 A2:A7 H2:I3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12">
-    <cfRule type="cellIs" dxfId="47" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:G7 C4:G6 G2">
-    <cfRule type="cellIs" dxfId="46" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="45" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="43" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="42" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="41" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5704,7 +5584,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="C5:G6"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5722,56 +5602,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150330</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>0.75</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="48">
         <f>AVERAGE(D4:F4)</f>
         <v>0.91666666666666663</v>
       </c>
@@ -5779,22 +5659,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="48">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5802,22 +5682,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="28" t="e">
+      <c r="G6" s="27" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5863,42 +5743,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:XFD7 A2:A7 H2:I3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12">
-    <cfRule type="cellIs" dxfId="40" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:G7 C4:G6 G2">
-    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="38" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5911,8 +5791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="C2:G7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5923,135 +5803,135 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="30">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="29">
         <v>150227</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150331</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="29">
         <v>150430</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="49">
         <v>0.88</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>2</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="49">
         <v>0.91</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>4</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="49">
         <v>0.88</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3 C2:E2 D4:G6 G2">
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="32" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="31" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="30" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7">
-    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Concentrado de metricas abril , actualizado por errores de escritura encontrados internamente
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150430.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150430.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -558,9 +558,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -582,6 +579,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1375,11 +1375,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345137904"/>
-        <c:axId val="345138464"/>
+        <c:axId val="411166784"/>
+        <c:axId val="411155024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345137904"/>
+        <c:axId val="411166784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1389,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345138464"/>
+        <c:crossAx val="411155024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345138464"/>
+        <c:axId val="411155024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1408,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345137904"/>
+        <c:crossAx val="411166784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,7 +1460,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1524,11 +1523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="398206688"/>
-        <c:axId val="398207248"/>
+        <c:axId val="319698256"/>
+        <c:axId val="319698816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="398206688"/>
+        <c:axId val="319698256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1537,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="398207248"/>
+        <c:crossAx val="319698816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1546,7 +1545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="398207248"/>
+        <c:axId val="319698816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1558,7 +1557,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="398206688"/>
+        <c:crossAx val="319698256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1782,11 +1781,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="398583264"/>
-        <c:axId val="295112224"/>
+        <c:axId val="436438848"/>
+        <c:axId val="436439408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="398583264"/>
+        <c:axId val="436438848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1796,7 +1795,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295112224"/>
+        <c:crossAx val="436439408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1804,7 +1803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295112224"/>
+        <c:axId val="436439408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1816,7 +1815,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="398583264"/>
+        <c:crossAx val="436438848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1988,11 +1987,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="290162272"/>
-        <c:axId val="290162832"/>
+        <c:axId val="411151104"/>
+        <c:axId val="411153904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290162272"/>
+        <c:axId val="411151104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +2001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290162832"/>
+        <c:crossAx val="411153904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2010,7 +2009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290162832"/>
+        <c:axId val="411153904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2023,7 +2022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290162272"/>
+        <c:crossAx val="411151104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2189,11 +2188,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="290165632"/>
-        <c:axId val="294236128"/>
+        <c:axId val="411158384"/>
+        <c:axId val="411159504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290165632"/>
+        <c:axId val="411158384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,7 +2202,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294236128"/>
+        <c:crossAx val="411159504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2211,7 +2210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294236128"/>
+        <c:axId val="411159504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2222,7 +2221,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290165632"/>
+        <c:crossAx val="411158384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2343,11 +2342,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="294238928"/>
-        <c:axId val="294239488"/>
+        <c:axId val="411161184"/>
+        <c:axId val="411160064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="294238928"/>
+        <c:axId val="411161184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,7 +2356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294239488"/>
+        <c:crossAx val="411160064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2365,7 +2364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294239488"/>
+        <c:axId val="411160064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2378,7 +2377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294238928"/>
+        <c:crossAx val="411161184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2425,7 +2424,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2489,11 +2487,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="296834528"/>
-        <c:axId val="296835088"/>
+        <c:axId val="411162864"/>
+        <c:axId val="411166224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296834528"/>
+        <c:axId val="411162864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,7 +2501,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296835088"/>
+        <c:crossAx val="411166224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2511,7 +2509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296835088"/>
+        <c:axId val="411166224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,7 +2520,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296834528"/>
+        <c:crossAx val="411162864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2575,7 +2573,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2639,11 +2636,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="294936480"/>
-        <c:axId val="294937040"/>
+        <c:axId val="319684816"/>
+        <c:axId val="319685376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="294936480"/>
+        <c:axId val="319684816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2653,7 +2650,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294937040"/>
+        <c:crossAx val="319685376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2661,7 +2658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294937040"/>
+        <c:axId val="319685376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2673,7 +2670,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294936480"/>
+        <c:crossAx val="319684816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,7 +2723,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2796,11 +2792,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104260080"/>
-        <c:axId val="104260640"/>
+        <c:axId val="319688176"/>
+        <c:axId val="319688736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104260080"/>
+        <c:axId val="319688176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2810,7 +2806,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104260640"/>
+        <c:crossAx val="319688736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2818,7 +2814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104260640"/>
+        <c:axId val="319688736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2830,7 +2826,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104260080"/>
+        <c:crossAx val="319688176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2883,7 +2879,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2947,11 +2942,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288223312"/>
-        <c:axId val="288223872"/>
+        <c:axId val="319691536"/>
+        <c:axId val="319692096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288223312"/>
+        <c:axId val="319691536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2961,7 +2956,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288223872"/>
+        <c:crossAx val="319692096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2969,7 +2964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288223872"/>
+        <c:axId val="319692096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2981,7 +2976,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288223312"/>
+        <c:crossAx val="319691536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3034,7 +3029,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3098,11 +3092,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288226672"/>
-        <c:axId val="398203888"/>
+        <c:axId val="319694896"/>
+        <c:axId val="319695456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288226672"/>
+        <c:axId val="319694896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3112,7 +3106,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="398203888"/>
+        <c:crossAx val="319695456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3120,7 +3114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="398203888"/>
+        <c:axId val="319695456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3132,7 +3126,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288226672"/>
+        <c:crossAx val="319694896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3175,7 +3169,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3211,7 +3205,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3254,7 +3248,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3292,7 +3286,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3335,7 +3329,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3371,7 +3365,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3412,7 +3406,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3448,7 +3442,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3489,7 +3483,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3532,7 +3526,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3880,7 +3874,7 @@
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3911,7 @@
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>0</v>
@@ -3930,7 +3924,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="49" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -3942,13 +3936,13 @@
       <c r="E20" s="37">
         <v>33</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="40">
         <f>(D20-E20)/D20</f>
         <v>0.63815789473684215</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
@@ -3958,13 +3952,13 @@
       <c r="E21" s="37">
         <v>13</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="41">
         <f t="shared" ref="F21:F26" si="0">(D21-E21)/D21</f>
         <v>0.71491228070175439</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -3976,13 +3970,13 @@
       <c r="E22" s="37">
         <v>17</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F22" s="40">
         <f t="shared" si="0"/>
         <v>0.62719298245614041</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
@@ -3992,7 +3986,7 @@
       <c r="E23" s="37">
         <v>28</v>
       </c>
-      <c r="F23" s="42">
+      <c r="F23" s="41">
         <f t="shared" si="0"/>
         <v>0.69298245614035092</v>
       </c>
@@ -4008,7 +4002,7 @@
       <c r="E24" s="36">
         <v>1</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="42">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
@@ -4024,7 +4018,7 @@
       <c r="E25" s="36">
         <v>1.6</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="42">
         <f t="shared" si="0"/>
         <v>0.19999999999999996</v>
       </c>
@@ -4040,7 +4034,7 @@
       <c r="E26" s="39">
         <v>0.17</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="43">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4548,8 +4542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,7 +4580,7 @@
     <row r="18" spans="2:5" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:5" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>0</v>
@@ -4608,7 +4602,7 @@
       <c r="D20" s="15">
         <v>1914.52</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="44">
         <f>(C20-D20)/C20</f>
         <v>0.80833717088797674</v>
       </c>
@@ -4623,7 +4617,7 @@
       <c r="D21" s="15">
         <v>1984.52</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="45">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.65145519720815703</v>
       </c>
@@ -4721,7 +4715,7 @@
       <c r="F4" s="22">
         <v>1</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4742,7 +4736,7 @@
       <c r="F5" s="22">
         <v>1</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>0.9</v>
       </c>
@@ -5022,7 +5016,7 @@
       <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="47">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5045,7 +5039,7 @@
       <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="47">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5068,7 +5062,7 @@
       <c r="F6" s="23">
         <v>1</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="47">
         <f>AVERAGE(D6:F6)</f>
         <v>1</v>
       </c>
@@ -5091,7 +5085,7 @@
       <c r="F7" s="23">
         <v>1</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="47">
         <f>AVERAGE(D7:F7)</f>
         <v>1</v>
       </c>
@@ -5443,7 +5437,7 @@
       <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="47">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5466,7 +5460,7 @@
       <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="47">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5651,7 +5645,7 @@
       <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="47">
         <f>AVERAGE(D4:F4)</f>
         <v>0.91666666666666663</v>
       </c>
@@ -5674,7 +5668,7 @@
       <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="47">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5791,7 +5785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -5839,7 +5833,7 @@
       <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="49">
+      <c r="G4" s="48">
         <v>0.88</v>
       </c>
     </row>
@@ -5856,7 +5850,7 @@
       <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="48">
         <v>0.91</v>
       </c>
     </row>
@@ -5873,7 +5867,7 @@
       <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5890,7 +5884,7 @@
       <c r="F7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="48">
         <v>0.88</v>
       </c>
     </row>

</xml_diff>